<commit_message>
- refactor import service  - added custom casters  - added future - static map for import  - fix tests
</commit_message>
<xml_diff>
--- a/tests/_data/reviews.xlsx
+++ b/tests/_data/reviews.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="review_test" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="reviews_test2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">b24StationId</t>
   </si>
@@ -41,6 +40,9 @@
     <t xml:space="preserve">Дата публикации</t>
   </si>
   <si>
+    <t xml:space="preserve">[138] Service Архангельск</t>
+  </si>
+  <si>
     <t xml:space="preserve">Отзыв</t>
   </si>
   <si>
@@ -50,6 +52,9 @@
     <t xml:space="preserve">Отзыв от клиента</t>
   </si>
   <si>
+    <t xml:space="preserve">[178] Service — Колпино</t>
+  </si>
+  <si>
     <t xml:space="preserve">Отзыв 2</t>
   </si>
   <si>
@@ -59,10 +64,10 @@
     <t xml:space="preserve">Кука доволен</t>
   </si>
   <si>
-    <t xml:space="preserve">Отзыв 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Бяка</t>
+    <t xml:space="preserve">Отзыв 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Бука</t>
   </si>
 </sst>
 </file>
@@ -164,19 +169,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.87"/>
   </cols>
   <sheetData>
@@ -201,17 +206,17 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>138</v>
+      <c r="A2" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>5</v>
@@ -221,17 +226,17 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>178</v>
+      <c r="A3" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>4.2</v>
@@ -239,6 +244,18 @@
       <c r="F3" s="1" t="n">
         <v>43580</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -249,72 +266,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.71"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>181</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>43580</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>